<commit_message>
#3495-PurchasenoInvoicePlan3 https://mobileapp.nstda.or.th/redmine/issues/3495 Module: pabi_account_report แก้ไขการดึงข้อมูลรายงานและเพิ่มข้อมูลในรายงาน
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>PO Number</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>to</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>WA Number</t>
+  </si>
+  <si>
+    <t>Recieive Quantity</t>
   </si>
 </sst>
 </file>
@@ -553,10 +565,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AY10"/>
+  <dimension ref="A1:BE10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+      <selection activeCell="AR16" sqref="AR16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -564,7 +576,7 @@
     <col min="1" max="1" width="24.375" customWidth="1"/>
     <col min="2" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="18.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.75" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.875" customWidth="1"/>
     <col min="7" max="7" width="23.875" customWidth="1"/>
     <col min="8" max="8" width="21.125" customWidth="1"/>
@@ -584,42 +596,51 @@
     <col min="22" max="22" width="28.625" customWidth="1"/>
     <col min="23" max="23" width="16.875" customWidth="1"/>
     <col min="24" max="24" width="16.375" customWidth="1"/>
-    <col min="25" max="25" width="16.125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.625" customWidth="1"/>
-    <col min="27" max="27" width="12.625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="12.125" customWidth="1"/>
-    <col min="30" max="30" width="11.125" customWidth="1"/>
-    <col min="31" max="31" width="12.625" customWidth="1"/>
-    <col min="32" max="32" width="12.75" customWidth="1"/>
-    <col min="33" max="33" width="14.125" customWidth="1"/>
-    <col min="34" max="34" width="14.75" customWidth="1"/>
-    <col min="35" max="35" width="16" customWidth="1"/>
-    <col min="36" max="36" width="15.875" customWidth="1"/>
-    <col min="37" max="37" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.625" customWidth="1"/>
-    <col min="39" max="39" width="16.375" customWidth="1"/>
-    <col min="40" max="40" width="16.75" customWidth="1"/>
-    <col min="41" max="41" width="12.25" customWidth="1"/>
-    <col min="42" max="43" width="13.625" customWidth="1"/>
-    <col min="44" max="44" width="19" customWidth="1"/>
-    <col min="45" max="46" width="16.625" customWidth="1"/>
+    <col min="25" max="26" width="19.5" customWidth="1"/>
+    <col min="27" max="27" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.625" customWidth="1"/>
+    <col min="29" max="29" width="16.25" style="1" customWidth="1"/>
+    <col min="30" max="30" width="17" style="1" customWidth="1"/>
+    <col min="31" max="31" width="17.5" customWidth="1"/>
+    <col min="32" max="32" width="11.125" customWidth="1"/>
+    <col min="33" max="33" width="12.625" customWidth="1"/>
+    <col min="34" max="34" width="12.75" customWidth="1"/>
+    <col min="35" max="35" width="17.125" customWidth="1"/>
+    <col min="36" max="36" width="15" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.875" customWidth="1"/>
+    <col min="38" max="38" width="19" customWidth="1"/>
+    <col min="39" max="39" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.375" customWidth="1"/>
+    <col min="41" max="41" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.5" customWidth="1"/>
+    <col min="43" max="44" width="18.5" customWidth="1"/>
+    <col min="45" max="45" width="17.875" customWidth="1"/>
+    <col min="46" max="46" width="16.75" customWidth="1"/>
+    <col min="47" max="47" width="13" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.375" customWidth="1"/>
+    <col min="50" max="50" width="21.625" customWidth="1"/>
+    <col min="51" max="51" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>48</v>
       </c>
       <c r="X2" s="1"/>
-      <c r="Y2"/>
+      <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA2"/>
+      <c r="AB2" s="1"/>
+    </row>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -630,26 +651,32 @@
         <v>53</v>
       </c>
       <c r="X3" s="1"/>
-      <c r="Y3"/>
+      <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA3"/>
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="X4" s="1"/>
-      <c r="Y4"/>
+      <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA4"/>
+      <c r="AB4" s="1"/>
+    </row>
+    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="X5" s="1"/>
-      <c r="Y5"/>
+      <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA5"/>
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
@@ -660,31 +687,39 @@
         <v>53</v>
       </c>
       <c r="X6" s="1"/>
-      <c r="Y6"/>
+      <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA6"/>
+      <c r="AB6" s="1"/>
+    </row>
+    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
       <c r="X7" s="1"/>
-      <c r="Y7"/>
+      <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA7"/>
+      <c r="AB7" s="1"/>
+    </row>
+    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="X8" s="1"/>
-      <c r="Y8"/>
+      <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
-    </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA8"/>
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
       <c r="X9" s="1"/>
-      <c r="Y9"/>
+      <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-    </row>
-    <row r="10" spans="1:51" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA9"/>
+      <c r="AB9" s="1"/>
+    </row>
+    <row r="10" spans="1:57" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -758,75 +793,93 @@
         <v>36</v>
       </c>
       <c r="Y10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Z10" s="4" t="s">
+      <c r="AB10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AA10" s="7" t="s">
+      <c r="AC10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AB10" s="7" t="s">
+      <c r="AD10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AC10" s="7" t="s">
+      <c r="AE10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AD10" s="4" t="s">
+      <c r="AF10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AE10" s="7" t="s">
+      <c r="AG10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AF10" s="7" t="s">
+      <c r="AH10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AG10" s="4" t="s">
+      <c r="AI10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AH10" s="7" t="s">
+      <c r="AJ10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AI10" s="4" t="s">
+      <c r="AK10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AJ10" s="4" t="s">
+      <c r="AL10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AK10" s="4" t="s">
+      <c r="AM10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AL10" s="4" t="s">
+      <c r="AN10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AM10" s="4" t="s">
+      <c r="AS10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AN10" s="4" t="s">
+      <c r="AT10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AO10" s="4" t="s">
+      <c r="AU10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AP10" s="4" t="s">
+      <c r="AV10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AQ10" s="4" t="s">
+      <c r="AW10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AR10" s="4" t="s">
+      <c r="AX10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AS10" s="4" t="s">
+      <c r="AY10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AT10" s="4" t="s">
+      <c r="AZ10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AU10" s="4" t="s">
+      <c r="BA10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AY10" s="4" t="s">
+      <c r="BE10" s="4" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#3495-PurchasenoInvoicePlan4 https://mobileapp.nstda.or.th/redmine/issues/3495 Module: pabi_account_report แก้ไขการดึงข้อมูลรายงานและเพิ่มข้อมูลในรายงาน
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\invoice\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>PO Number</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>to</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>WA Number</t>
+  </si>
+  <si>
+    <t>Recieive Quantity</t>
   </si>
 </sst>
 </file>
@@ -553,10 +565,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AY10"/>
+  <dimension ref="A1:BE10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+      <selection activeCell="AR16" sqref="AR16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -564,7 +576,7 @@
     <col min="1" max="1" width="24.375" customWidth="1"/>
     <col min="2" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="18.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.75" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.875" customWidth="1"/>
     <col min="7" max="7" width="23.875" customWidth="1"/>
     <col min="8" max="8" width="21.125" customWidth="1"/>
@@ -584,42 +596,51 @@
     <col min="22" max="22" width="28.625" customWidth="1"/>
     <col min="23" max="23" width="16.875" customWidth="1"/>
     <col min="24" max="24" width="16.375" customWidth="1"/>
-    <col min="25" max="25" width="16.125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.625" customWidth="1"/>
-    <col min="27" max="27" width="12.625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="12.125" customWidth="1"/>
-    <col min="30" max="30" width="11.125" customWidth="1"/>
-    <col min="31" max="31" width="12.625" customWidth="1"/>
-    <col min="32" max="32" width="12.75" customWidth="1"/>
-    <col min="33" max="33" width="14.125" customWidth="1"/>
-    <col min="34" max="34" width="14.75" customWidth="1"/>
-    <col min="35" max="35" width="16" customWidth="1"/>
-    <col min="36" max="36" width="15.875" customWidth="1"/>
-    <col min="37" max="37" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.625" customWidth="1"/>
-    <col min="39" max="39" width="16.375" customWidth="1"/>
-    <col min="40" max="40" width="16.75" customWidth="1"/>
-    <col min="41" max="41" width="12.25" customWidth="1"/>
-    <col min="42" max="43" width="13.625" customWidth="1"/>
-    <col min="44" max="44" width="19" customWidth="1"/>
-    <col min="45" max="46" width="16.625" customWidth="1"/>
+    <col min="25" max="26" width="19.5" customWidth="1"/>
+    <col min="27" max="27" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.625" customWidth="1"/>
+    <col min="29" max="29" width="16.25" style="1" customWidth="1"/>
+    <col min="30" max="30" width="17" style="1" customWidth="1"/>
+    <col min="31" max="31" width="17.5" customWidth="1"/>
+    <col min="32" max="32" width="11.125" customWidth="1"/>
+    <col min="33" max="33" width="12.625" customWidth="1"/>
+    <col min="34" max="34" width="12.75" customWidth="1"/>
+    <col min="35" max="35" width="17.125" customWidth="1"/>
+    <col min="36" max="36" width="15" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.875" customWidth="1"/>
+    <col min="38" max="38" width="19" customWidth="1"/>
+    <col min="39" max="39" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="16.375" customWidth="1"/>
+    <col min="41" max="41" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.5" customWidth="1"/>
+    <col min="43" max="44" width="18.5" customWidth="1"/>
+    <col min="45" max="45" width="17.875" customWidth="1"/>
+    <col min="46" max="46" width="16.75" customWidth="1"/>
+    <col min="47" max="47" width="13" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="22.375" customWidth="1"/>
+    <col min="50" max="50" width="21.625" customWidth="1"/>
+    <col min="51" max="51" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>48</v>
       </c>
       <c r="X2" s="1"/>
-      <c r="Y2"/>
+      <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA2"/>
+      <c r="AB2" s="1"/>
+    </row>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -630,26 +651,32 @@
         <v>53</v>
       </c>
       <c r="X3" s="1"/>
-      <c r="Y3"/>
+      <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA3"/>
+      <c r="AB3" s="1"/>
+    </row>
+    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="X4" s="1"/>
-      <c r="Y4"/>
+      <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
-    </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA4"/>
+      <c r="AB4" s="1"/>
+    </row>
+    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="X5" s="1"/>
-      <c r="Y5"/>
+      <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
-    </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA5"/>
+      <c r="AB5" s="1"/>
+    </row>
+    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
@@ -660,31 +687,39 @@
         <v>53</v>
       </c>
       <c r="X6" s="1"/>
-      <c r="Y6"/>
+      <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA6"/>
+      <c r="AB6" s="1"/>
+    </row>
+    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
       <c r="X7" s="1"/>
-      <c r="Y7"/>
+      <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
-    </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA7"/>
+      <c r="AB7" s="1"/>
+    </row>
+    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="X8" s="1"/>
-      <c r="Y8"/>
+      <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
-    </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
+      <c r="AA8"/>
+      <c r="AB8" s="1"/>
+    </row>
+    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
       <c r="X9" s="1"/>
-      <c r="Y9"/>
+      <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-    </row>
-    <row r="10" spans="1:51" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AA9"/>
+      <c r="AB9" s="1"/>
+    </row>
+    <row r="10" spans="1:57" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -758,75 +793,93 @@
         <v>36</v>
       </c>
       <c r="Y10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Z10" s="4" t="s">
+      <c r="AB10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AA10" s="7" t="s">
+      <c r="AC10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AB10" s="7" t="s">
+      <c r="AD10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AC10" s="7" t="s">
+      <c r="AE10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AD10" s="4" t="s">
+      <c r="AF10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AE10" s="7" t="s">
+      <c r="AG10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AF10" s="7" t="s">
+      <c r="AH10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AG10" s="4" t="s">
+      <c r="AI10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AH10" s="7" t="s">
+      <c r="AJ10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AI10" s="4" t="s">
+      <c r="AK10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AJ10" s="4" t="s">
+      <c r="AL10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AK10" s="4" t="s">
+      <c r="AM10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AL10" s="4" t="s">
+      <c r="AN10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AQ10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AR10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AM10" s="4" t="s">
+      <c r="AS10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AN10" s="4" t="s">
+      <c r="AT10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AO10" s="4" t="s">
+      <c r="AU10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AP10" s="4" t="s">
+      <c r="AV10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AQ10" s="4" t="s">
+      <c r="AW10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AR10" s="4" t="s">
+      <c r="AX10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AS10" s="4" t="s">
+      <c r="AY10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AT10" s="4" t="s">
+      <c r="AZ10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AU10" s="4" t="s">
+      <c r="BA10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AY10" s="4" t="s">
+      <c r="BE10" s="4" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#3386&3495-PurchaseInvoicePlan Module: pabi_account_report แก้ไข template รายงานและการดึงข้อมูลออกรายงาน https://mobileapp.nstda.or.th/redmine/issues/3386 https://mobileapp.nstda.or.th/redmine/issues/3495
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\111\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>PO Number</t>
   </si>
@@ -186,6 +186,21 @@
   </si>
   <si>
     <t>to</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Unit Price</t>
+  </si>
+  <si>
+    <t>WA Number</t>
+  </si>
+  <si>
+    <t>Recieive Quantity</t>
+  </si>
+  <si>
+    <t>INV.Plan Description</t>
   </si>
 </sst>
 </file>
@@ -553,18 +568,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AY10"/>
+  <dimension ref="A1:BF10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.375" customWidth="1"/>
     <col min="2" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="18.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.75" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.875" customWidth="1"/>
     <col min="7" max="7" width="23.875" customWidth="1"/>
     <col min="8" max="8" width="21.125" customWidth="1"/>
@@ -584,42 +597,53 @@
     <col min="22" max="22" width="28.625" customWidth="1"/>
     <col min="23" max="23" width="16.875" customWidth="1"/>
     <col min="24" max="24" width="16.375" customWidth="1"/>
-    <col min="25" max="25" width="16.125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="12.625" customWidth="1"/>
-    <col min="27" max="27" width="12.625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="12.125" customWidth="1"/>
-    <col min="30" max="30" width="11.125" customWidth="1"/>
-    <col min="31" max="31" width="12.625" customWidth="1"/>
-    <col min="32" max="32" width="12.75" customWidth="1"/>
-    <col min="33" max="33" width="14.125" customWidth="1"/>
-    <col min="34" max="34" width="14.75" customWidth="1"/>
-    <col min="35" max="35" width="16" customWidth="1"/>
-    <col min="36" max="36" width="15.875" customWidth="1"/>
-    <col min="37" max="37" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.625" customWidth="1"/>
-    <col min="39" max="39" width="16.375" customWidth="1"/>
-    <col min="40" max="40" width="16.75" customWidth="1"/>
-    <col min="41" max="41" width="12.25" customWidth="1"/>
-    <col min="42" max="43" width="13.625" customWidth="1"/>
-    <col min="44" max="44" width="19" customWidth="1"/>
-    <col min="45" max="46" width="16.625" customWidth="1"/>
+    <col min="25" max="26" width="19.5" customWidth="1"/>
+    <col min="27" max="27" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="25.125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="12.625" customWidth="1"/>
+    <col min="30" max="30" width="16.25" style="1" customWidth="1"/>
+    <col min="31" max="31" width="17" style="1" customWidth="1"/>
+    <col min="32" max="32" width="17.5" customWidth="1"/>
+    <col min="33" max="33" width="11.125" customWidth="1"/>
+    <col min="34" max="34" width="12.625" customWidth="1"/>
+    <col min="35" max="35" width="12.75" customWidth="1"/>
+    <col min="36" max="36" width="17.125" customWidth="1"/>
+    <col min="37" max="37" width="15" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.875" customWidth="1"/>
+    <col min="39" max="39" width="19" customWidth="1"/>
+    <col min="40" max="40" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.375" customWidth="1"/>
+    <col min="42" max="42" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.5" customWidth="1"/>
+    <col min="44" max="45" width="18.5" customWidth="1"/>
+    <col min="46" max="46" width="17.875" customWidth="1"/>
+    <col min="47" max="47" width="16.75" customWidth="1"/>
+    <col min="48" max="48" width="13" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="24.75" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="22.375" customWidth="1"/>
+    <col min="51" max="51" width="21.625" customWidth="1"/>
+    <col min="52" max="52" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>48</v>
       </c>
       <c r="X2" s="1"/>
-      <c r="Y2"/>
+      <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2" s="1"/>
     </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -630,26 +654,35 @@
         <v>53</v>
       </c>
       <c r="X3" s="1"/>
-      <c r="Y3"/>
+      <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="X4" s="1"/>
-      <c r="Y4"/>
+      <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="X5" s="1"/>
-      <c r="Y5"/>
+      <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>39</v>
       </c>
@@ -660,31 +693,43 @@
         <v>53</v>
       </c>
       <c r="X6" s="1"/>
-      <c r="Y6"/>
+      <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
+      <c r="AA6"/>
+      <c r="AB6"/>
+      <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>50</v>
       </c>
       <c r="X7" s="1"/>
-      <c r="Y7"/>
+      <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
+      <c r="AA7"/>
+      <c r="AB7"/>
+      <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="X8" s="1"/>
-      <c r="Y8"/>
+      <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
       <c r="X9" s="1"/>
-      <c r="Y9"/>
+      <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
+      <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:51" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -758,75 +803,96 @@
         <v>36</v>
       </c>
       <c r="Y10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="Z10" s="4" t="s">
+      <c r="AB10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="AA10" s="7" t="s">
+      <c r="AD10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AB10" s="7" t="s">
+      <c r="AE10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AC10" s="7" t="s">
+      <c r="AF10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="AD10" s="4" t="s">
+      <c r="AG10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AE10" s="7" t="s">
+      <c r="AH10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="AF10" s="7" t="s">
+      <c r="AI10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AG10" s="4" t="s">
+      <c r="AJ10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AH10" s="7" t="s">
+      <c r="AK10" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AI10" s="4" t="s">
+      <c r="AL10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AJ10" s="4" t="s">
+      <c r="AM10" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AK10" s="4" t="s">
+      <c r="AN10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AL10" s="4" t="s">
+      <c r="AO10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AQ10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS10" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AM10" s="4" t="s">
+      <c r="AT10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AN10" s="4" t="s">
+      <c r="AU10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AO10" s="4" t="s">
+      <c r="AV10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AP10" s="4" t="s">
+      <c r="AW10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AQ10" s="4" t="s">
+      <c r="AX10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AR10" s="4" t="s">
+      <c r="AY10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AS10" s="4" t="s">
+      <c r="AZ10" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AT10" s="4" t="s">
+      <c r="BA10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AU10" s="4" t="s">
+      <c r="BB10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AY10" s="4" t="s">
+      <c r="BF10" s="4" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#3724-InvoicePlan Module: pabi_account_report https://mobileapp.nstda.or.th/redmine/issues/3724 แก้ query และเพิ่ม column ใน excel
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\111\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\xls file\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>PO Number</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Contract End Date</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Installment</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Fund</t>
   </si>
   <si>
-    <t>Exchange Rate</t>
-  </si>
-  <si>
     <t xml:space="preserve">Amount </t>
   </si>
   <si>
@@ -201,6 +195,24 @@
   </si>
   <si>
     <t>INV.Plan Description</t>
+  </si>
+  <si>
+    <t>Exchange Rate PO</t>
+  </si>
+  <si>
+    <t>Acceptance Date</t>
+  </si>
+  <si>
+    <t>Exchange Rate KV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PO State </t>
+  </si>
+  <si>
+    <t>PO Close</t>
+  </si>
+  <si>
+    <t>InvoicePlan status</t>
   </si>
 </sst>
 </file>
@@ -568,9 +580,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BF10"/>
+  <dimension ref="A1:BG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -627,14 +641,14 @@
     <col min="54" max="54" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -643,15 +657,15 @@
       <c r="AB2"/>
       <c r="AC2" s="1"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
@@ -660,7 +674,7 @@
       <c r="AB3"/>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -671,7 +685,7 @@
       <c r="AB4"/>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -682,15 +696,15 @@
       <c r="AB5"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
@@ -699,9 +713,9 @@
       <c r="AB6"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
@@ -710,7 +724,7 @@
       <c r="AB7"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -721,7 +735,7 @@
       <c r="AB8"/>
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.2">
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -729,7 +743,7 @@
       <c r="AB9"/>
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -752,10 +766,10 @@
         <v>29</v>
       </c>
       <c r="H10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>13</v>
@@ -764,10 +778,10 @@
         <v>31</v>
       </c>
       <c r="L10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="N10" s="4" t="s">
         <v>27</v>
@@ -779,10 +793,10 @@
         <v>20</v>
       </c>
       <c r="Q10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="S10" s="4" t="s">
         <v>22</v>
@@ -797,22 +811,22 @@
         <v>25</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Z10" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB10" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="AC10" s="4" t="s">
         <v>2</v>
@@ -821,7 +835,7 @@
         <v>28</v>
       </c>
       <c r="AE10" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AF10" s="7" t="s">
         <v>5</v>
@@ -833,13 +847,13 @@
         <v>7</v>
       </c>
       <c r="AI10" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AJ10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="AK10" s="7" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="AL10" s="4" t="s">
         <v>15</v>
@@ -851,49 +865,61 @@
         <v>9</v>
       </c>
       <c r="AO10" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="AP10" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AQ10" s="4" t="s">
         <v>55</v>
       </c>
       <c r="AR10" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AS10" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="AT10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AU10" s="4" t="s">
+      <c r="AV10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AV10" s="4" t="s">
+      <c r="AW10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AW10" s="4" t="s">
+      <c r="AX10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AX10" s="4" t="s">
+      <c r="AY10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AZ10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="BA10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BC10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AY10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AZ10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="BB10" s="4" t="s">
+      <c r="BD10" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="BE10" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="BF10" s="4" t="s">
-        <v>32</v>
+        <v>61</v>
+      </c>
+      <c r="BG10" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#3724-InvoicePlan&SpecialCharacter Module: pabi_account_report,pabi_utils https://mobileapp.nstda.or.th/redmine/issues/3724 - เพิ่มช่อง Purchase Invoice Plan and Purchase No invoice Plan ในรายงาน - แก้ไข SpecialCharacter
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\111\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aommy\pabi_file\000\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>PO Number</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Contract End Date</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Installment</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Fund</t>
   </si>
   <si>
-    <t>Exchange Rate</t>
-  </si>
-  <si>
     <t xml:space="preserve">Amount </t>
   </si>
   <si>
@@ -182,12 +176,6 @@
     <t>Deposit</t>
   </si>
   <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -201,6 +189,24 @@
   </si>
   <si>
     <t>INV.Plan Description</t>
+  </si>
+  <si>
+    <t>Exchange Rate PO</t>
+  </si>
+  <si>
+    <t>Acceptance Date</t>
+  </si>
+  <si>
+    <t>Exchange Rate KV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PO State </t>
+  </si>
+  <si>
+    <t>PO Close</t>
+  </si>
+  <si>
+    <t>InvoicePlan status</t>
   </si>
 </sst>
 </file>
@@ -270,7 +276,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -278,11 +284,18 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma 5 2" xfId="2"/>
@@ -568,73 +581,57 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BF10"/>
+  <dimension ref="A1:BG10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.375" customWidth="1"/>
-    <col min="2" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="18.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.875" customWidth="1"/>
-    <col min="7" max="7" width="23.875" customWidth="1"/>
-    <col min="8" max="8" width="21.125" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="15.625" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="16.375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="29.875" customWidth="1"/>
-    <col min="14" max="14" width="16.75" customWidth="1"/>
-    <col min="15" max="15" width="22.75" customWidth="1"/>
-    <col min="16" max="16" width="30.625" customWidth="1"/>
-    <col min="17" max="17" width="13.875" customWidth="1"/>
-    <col min="18" max="18" width="34.875" customWidth="1"/>
-    <col min="19" max="19" width="25.75" customWidth="1"/>
-    <col min="20" max="20" width="15.875" customWidth="1"/>
-    <col min="21" max="21" width="16" customWidth="1"/>
-    <col min="22" max="22" width="28.625" customWidth="1"/>
-    <col min="23" max="23" width="16.875" customWidth="1"/>
-    <col min="24" max="24" width="16.375" customWidth="1"/>
-    <col min="25" max="26" width="19.5" customWidth="1"/>
-    <col min="27" max="27" width="11.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="25.125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="12.625" customWidth="1"/>
-    <col min="30" max="30" width="16.25" style="1" customWidth="1"/>
-    <col min="31" max="31" width="17" style="1" customWidth="1"/>
-    <col min="32" max="32" width="17.5" customWidth="1"/>
-    <col min="33" max="33" width="11.125" customWidth="1"/>
-    <col min="34" max="34" width="12.625" customWidth="1"/>
-    <col min="35" max="35" width="12.75" customWidth="1"/>
-    <col min="36" max="36" width="17.125" customWidth="1"/>
-    <col min="37" max="37" width="15" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.875" customWidth="1"/>
-    <col min="39" max="39" width="19" customWidth="1"/>
-    <col min="40" max="40" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.375" customWidth="1"/>
-    <col min="42" max="42" width="18.125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.5" customWidth="1"/>
-    <col min="44" max="45" width="18.5" customWidth="1"/>
-    <col min="46" max="46" width="17.875" customWidth="1"/>
-    <col min="47" max="47" width="16.75" customWidth="1"/>
-    <col min="48" max="48" width="13" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="22.375" customWidth="1"/>
-    <col min="51" max="51" width="21.625" customWidth="1"/>
-    <col min="52" max="52" width="8.25" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="12.875" customWidth="1"/>
+    <col min="3" max="3" width="16.25" customWidth="1"/>
+    <col min="4" max="4" width="16.25" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.875" customWidth="1"/>
+    <col min="6" max="6" width="16.25" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="16.25" customWidth="1"/>
+    <col min="9" max="9" width="23.375" customWidth="1"/>
+    <col min="10" max="11" width="16.25" customWidth="1"/>
+    <col min="12" max="12" width="16.25" style="2" customWidth="1"/>
+    <col min="13" max="18" width="42.375" customWidth="1"/>
+    <col min="19" max="19" width="16.25" customWidth="1"/>
+    <col min="20" max="20" width="42.375" customWidth="1"/>
+    <col min="21" max="21" width="16.25" customWidth="1"/>
+    <col min="22" max="23" width="42.375" customWidth="1"/>
+    <col min="24" max="24" width="14.75" customWidth="1"/>
+    <col min="25" max="25" width="13" customWidth="1"/>
+    <col min="26" max="26" width="16.25" customWidth="1"/>
+    <col min="27" max="27" width="12.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="42.375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="16.25" customWidth="1"/>
+    <col min="30" max="31" width="16.25" style="1" customWidth="1"/>
+    <col min="32" max="41" width="16.25" customWidth="1"/>
+    <col min="42" max="42" width="16.625" customWidth="1"/>
+    <col min="43" max="43" width="17.875" customWidth="1"/>
+    <col min="44" max="49" width="16.25" customWidth="1"/>
+    <col min="50" max="50" width="21.875" customWidth="1"/>
+    <col min="51" max="51" width="17.875" customWidth="1"/>
+    <col min="52" max="53" width="16.25" customWidth="1"/>
+    <col min="54" max="54" width="9.875" customWidth="1"/>
+    <col min="55" max="55" width="23" customWidth="1"/>
+    <col min="56" max="56" width="10.25" customWidth="1"/>
+    <col min="57" max="57" width="16.25" customWidth="1"/>
+    <col min="58" max="58" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -643,16 +640,12 @@
       <c r="AB2"/>
       <c r="AC2" s="1"/>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
+      <c r="D3"/>
+      <c r="E3" s="3"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
@@ -660,10 +653,12 @@
       <c r="AB3"/>
       <c r="AC3" s="1"/>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="D4"/>
+      <c r="E4" s="3"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
@@ -671,10 +666,12 @@
       <c r="AB4"/>
       <c r="AC4" s="1"/>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="D5"/>
+      <c r="E5" s="3"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
@@ -682,16 +679,12 @@
       <c r="AB5"/>
       <c r="AC5" s="1"/>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6" s="3"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
@@ -699,9 +692,9 @@
       <c r="AB6"/>
       <c r="AC6" s="1"/>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
@@ -710,7 +703,7 @@
       <c r="AB7"/>
       <c r="AC7" s="1"/>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -721,7 +714,7 @@
       <c r="AB8"/>
       <c r="AC8" s="1"/>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" x14ac:dyDescent="0.2">
       <c r="X9" s="1"/>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -729,171 +722,183 @@
       <c r="AB9"/>
       <c r="AC9" s="1"/>
     </row>
-    <row r="10" spans="1:58" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:59" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="J10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="V10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="X10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AH10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="R10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="T10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="U10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="V10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="W10" s="4" t="s">
+      <c r="AJ10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK10" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AM10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="AO10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="AQ10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AT10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AU10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AV10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AW10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AX10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AY10" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="X10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y10" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB10" s="4" t="s">
+      <c r="BA10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="BC10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="BD10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AC10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AE10" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AF10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AH10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="AI10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AK10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AO10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AP10" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AQ10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AR10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AS10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AT10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="AU10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="AV10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AW10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="AX10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AY10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AZ10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="BB10" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="BF10" s="4" t="s">
-        <v>32</v>
+      <c r="BF10" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="BG10" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#4126-PurchaseInvoicePlanReport Module: pabi_account_report **แก้ไข query และเพิ่มข้อมูลในรายงาน (Purchase Invoice Plan) https://mobileapp.nstda.or.th/redmine/issues/4126
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
   <si>
     <t>PO Number</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>InvoicePlan status</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>No. of Installment</t>
+  </si>
+  <si>
+    <t>Amount in Current Fiscal Year</t>
+  </si>
+  <si>
+    <t>Amount in Next Fiscal Year</t>
   </si>
 </sst>
 </file>
@@ -581,9 +593,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BG10"/>
+  <dimension ref="A1:BK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -592,137 +606,148 @@
     <col min="3" max="3" width="16.25" customWidth="1"/>
     <col min="4" max="4" width="16.25" style="3" customWidth="1"/>
     <col min="5" max="5" width="8.875" customWidth="1"/>
-    <col min="6" max="6" width="16.25" customWidth="1"/>
-    <col min="7" max="7" width="21.5" customWidth="1"/>
-    <col min="8" max="8" width="16.25" customWidth="1"/>
-    <col min="9" max="9" width="23.375" customWidth="1"/>
-    <col min="10" max="11" width="16.25" customWidth="1"/>
-    <col min="12" max="12" width="16.25" style="2" customWidth="1"/>
-    <col min="13" max="18" width="42.375" customWidth="1"/>
-    <col min="19" max="19" width="16.25" customWidth="1"/>
-    <col min="20" max="20" width="42.375" customWidth="1"/>
-    <col min="21" max="21" width="16.25" customWidth="1"/>
-    <col min="22" max="23" width="42.375" customWidth="1"/>
-    <col min="24" max="24" width="14.75" customWidth="1"/>
-    <col min="25" max="25" width="13" customWidth="1"/>
-    <col min="26" max="26" width="16.25" customWidth="1"/>
-    <col min="27" max="27" width="12.5" style="1" customWidth="1"/>
-    <col min="28" max="28" width="42.375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="16.25" customWidth="1"/>
-    <col min="30" max="31" width="16.25" style="1" customWidth="1"/>
-    <col min="32" max="41" width="16.25" customWidth="1"/>
-    <col min="42" max="42" width="16.625" customWidth="1"/>
-    <col min="43" max="43" width="17.875" customWidth="1"/>
-    <col min="44" max="49" width="16.25" customWidth="1"/>
-    <col min="50" max="50" width="21.875" customWidth="1"/>
-    <col min="51" max="51" width="17.875" customWidth="1"/>
-    <col min="52" max="53" width="16.25" customWidth="1"/>
-    <col min="54" max="54" width="9.875" customWidth="1"/>
-    <col min="55" max="55" width="23" customWidth="1"/>
-    <col min="56" max="56" width="10.25" customWidth="1"/>
-    <col min="57" max="57" width="16.25" customWidth="1"/>
-    <col min="58" max="58" width="9.75" customWidth="1"/>
+    <col min="6" max="7" width="16.25" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="16.25" customWidth="1"/>
+    <col min="10" max="10" width="23.375" customWidth="1"/>
+    <col min="11" max="12" width="16.25" customWidth="1"/>
+    <col min="13" max="13" width="16.25" style="2" customWidth="1"/>
+    <col min="14" max="19" width="42.375" customWidth="1"/>
+    <col min="20" max="20" width="16.25" customWidth="1"/>
+    <col min="21" max="21" width="42.375" customWidth="1"/>
+    <col min="22" max="22" width="16.25" customWidth="1"/>
+    <col min="23" max="24" width="42.375" customWidth="1"/>
+    <col min="25" max="25" width="14.75" customWidth="1"/>
+    <col min="26" max="26" width="13" customWidth="1"/>
+    <col min="27" max="27" width="16.25" customWidth="1"/>
+    <col min="28" max="28" width="13.875" customWidth="1"/>
+    <col min="29" max="29" width="12.5" style="1" customWidth="1"/>
+    <col min="30" max="30" width="42.375" style="1" customWidth="1"/>
+    <col min="31" max="31" width="16.25" customWidth="1"/>
+    <col min="32" max="33" width="16.25" style="1" customWidth="1"/>
+    <col min="34" max="41" width="16.25" customWidth="1"/>
+    <col min="42" max="43" width="19.5" customWidth="1"/>
+    <col min="44" max="45" width="16.25" customWidth="1"/>
+    <col min="46" max="46" width="16.625" customWidth="1"/>
+    <col min="47" max="47" width="17.875" customWidth="1"/>
+    <col min="48" max="53" width="16.25" customWidth="1"/>
+    <col min="54" max="54" width="21.875" customWidth="1"/>
+    <col min="55" max="55" width="17.875" customWidth="1"/>
+    <col min="56" max="57" width="16.25" customWidth="1"/>
+    <col min="58" max="58" width="9.875" customWidth="1"/>
+    <col min="59" max="59" width="23" customWidth="1"/>
+    <col min="60" max="60" width="10.25" customWidth="1"/>
+    <col min="61" max="61" width="16.25" customWidth="1"/>
+    <col min="62" max="62" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-      <c r="AA2"/>
-      <c r="AB2"/>
-      <c r="AC2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2" s="1"/>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D3"/>
       <c r="E3" s="3"/>
-      <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3"/>
-      <c r="AB3"/>
-      <c r="AC3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3" s="1"/>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D4"/>
       <c r="E4" s="3"/>
-      <c r="X4" s="1"/>
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
-      <c r="AA4"/>
-      <c r="AB4"/>
-      <c r="AC4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="3"/>
-      <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
-      <c r="AA5"/>
-      <c r="AB5"/>
-      <c r="AC5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D6"/>
       <c r="E6" s="3"/>
-      <c r="X6" s="1"/>
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
-      <c r="AA6"/>
-      <c r="AB6"/>
-      <c r="AC6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6"/>
+      <c r="AD6"/>
+      <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="X7" s="1"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
-      <c r="AA7"/>
-      <c r="AB7"/>
-      <c r="AC7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="X8" s="1"/>
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
-      <c r="AA8"/>
-      <c r="AB8"/>
-      <c r="AC8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:59" x14ac:dyDescent="0.2">
-      <c r="X9" s="1"/>
+    <row r="9" spans="1:63" x14ac:dyDescent="0.2">
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-      <c r="AC9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:59" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:63" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -742,162 +767,174 @@
         <v>30</v>
       </c>
       <c r="G10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="L10" s="5" t="s">
+      <c r="M10" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="5" t="s">
+      <c r="N10" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="O10" s="5" t="s">
+      <c r="P10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="Q10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="Q10" s="5" t="s">
+      <c r="R10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R10" s="5" t="s">
+      <c r="S10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="S10" s="5" t="s">
+      <c r="T10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="T10" s="5" t="s">
+      <c r="U10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="U10" s="5" t="s">
+      <c r="V10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="V10" s="5" t="s">
+      <c r="W10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="W10" s="5" t="s">
+      <c r="X10" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="X10" s="5" t="s">
+      <c r="Y10" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Y10" s="5" t="s">
+      <c r="Z10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="Z10" s="5" t="s">
+      <c r="AA10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AA10" s="5" t="s">
+      <c r="AB10" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AB10" s="5" t="s">
+      <c r="AD10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AC10" s="5" t="s">
+      <c r="AE10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AD10" s="8" t="s">
+      <c r="AF10" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AE10" s="8" t="s">
+      <c r="AG10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="AF10" s="8" t="s">
+      <c r="AH10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AG10" s="5" t="s">
+      <c r="AI10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AH10" s="8" t="s">
+      <c r="AJ10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AI10" s="8" t="s">
+      <c r="AK10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AJ10" s="5" t="s">
+      <c r="AL10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AK10" s="8" t="s">
+      <c r="AM10" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AL10" s="5" t="s">
+      <c r="AN10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AM10" s="5" t="s">
+      <c r="AO10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AN10" s="5" t="s">
+      <c r="AP10" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AO10" s="5" t="s">
+      <c r="AS10" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AP10" s="5" t="s">
+      <c r="AT10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AQ10" s="5" t="s">
+      <c r="AU10" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="AR10" s="5" t="s">
+      <c r="AV10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AS10" s="5" t="s">
+      <c r="AW10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AT10" s="5" t="s">
+      <c r="AX10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AU10" s="5" t="s">
+      <c r="AY10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AV10" s="5" t="s">
+      <c r="AZ10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AW10" s="5" t="s">
+      <c r="BA10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AX10" s="5" t="s">
+      <c r="BB10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="AY10" s="5" t="s">
+      <c r="BC10" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AZ10" s="5" t="s">
+      <c r="BD10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="BA10" s="5" t="s">
+      <c r="BE10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="BB10" s="5" t="s">
+      <c r="BF10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="BC10" s="5" t="s">
+      <c r="BG10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="BD10" s="5" t="s">
+      <c r="BH10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="BE10" s="5" t="s">
+      <c r="BI10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="BF10" s="5" t="s">
+      <c r="BJ10" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="BG10" s="5" t="s">
+      <c r="BK10" s="5" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#4285-PurchaseInvoiceReport Module: pabi_account_report (Restart&Update Module) *เพิ่ม Filter สำหรับออกรายงาน https://mobileapp.nstda.or.th/redmine/issues/4285
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>PO Number</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Subtotal</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>PO Contract</t>
   </si>
   <si>
@@ -219,6 +216,15 @@
   </si>
   <si>
     <t>Amount in Next Fiscal Year</t>
+  </si>
+  <si>
+    <t>Invoice Status</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Filter</t>
   </si>
 </sst>
 </file>
@@ -593,11 +599,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BK10"/>
+  <dimension ref="A1:BL11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -630,25 +634,25 @@
     <col min="44" max="45" width="16.25" customWidth="1"/>
     <col min="46" max="46" width="16.625" customWidth="1"/>
     <col min="47" max="47" width="17.875" customWidth="1"/>
-    <col min="48" max="53" width="16.25" customWidth="1"/>
-    <col min="54" max="54" width="21.875" customWidth="1"/>
-    <col min="55" max="55" width="17.875" customWidth="1"/>
-    <col min="56" max="57" width="16.25" customWidth="1"/>
-    <col min="58" max="58" width="9.875" customWidth="1"/>
-    <col min="59" max="59" width="23" customWidth="1"/>
-    <col min="60" max="60" width="10.25" customWidth="1"/>
-    <col min="61" max="61" width="16.25" customWidth="1"/>
-    <col min="62" max="62" width="9.75" customWidth="1"/>
+    <col min="48" max="54" width="16.25" customWidth="1"/>
+    <col min="55" max="55" width="21.875" customWidth="1"/>
+    <col min="56" max="56" width="17.875" customWidth="1"/>
+    <col min="57" max="58" width="16.25" customWidth="1"/>
+    <col min="59" max="59" width="9.875" customWidth="1"/>
+    <col min="60" max="60" width="23" customWidth="1"/>
+    <col min="61" max="61" width="10.25" customWidth="1"/>
+    <col min="62" max="62" width="16.25" customWidth="1"/>
+    <col min="63" max="63" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
@@ -658,9 +662,9 @@
       <c r="AD2"/>
       <c r="AE2" s="1"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3"/>
       <c r="E3" s="3"/>
@@ -672,7 +676,7 @@
       <c r="AD3"/>
       <c r="AE3" s="1"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -686,9 +690,9 @@
       <c r="AD4"/>
       <c r="AE4" s="1"/>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="3"/>
@@ -700,9 +704,9 @@
       <c r="AD5"/>
       <c r="AE5" s="1"/>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6"/>
       <c r="E6" s="3"/>
@@ -714,9 +718,9 @@
       <c r="AD6"/>
       <c r="AE6" s="1"/>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
@@ -726,7 +730,7 @@
       <c r="AD7"/>
       <c r="AE7" s="1"/>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -738,7 +742,10 @@
       <c r="AD8"/>
       <c r="AE8" s="1"/>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>66</v>
+      </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1"/>
@@ -747,198 +754,211 @@
       <c r="AD9"/>
       <c r="AE9" s="1"/>
     </row>
-    <row r="10" spans="1:63" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10"/>
+      <c r="AD10"/>
+      <c r="AE10" s="1"/>
+    </row>
+    <row r="11" spans="1:64" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="X11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB11" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG11" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="AK11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AL11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AP11" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR11" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="AX11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AY11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AZ11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB11" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="BC11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q10" s="7" t="s">
+      <c r="BD11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="BE11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="BF11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="BG11" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="BH11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="BI11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="R10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="S10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="U10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="V10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="W10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="X10" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB10" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF10" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG10" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH10" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="AK10" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AM10" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="AN10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="AO10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="AP10" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AQ10" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="AS10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AT10" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="AU10" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AV10" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AW10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AX10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AY10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AZ10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="BA10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="BB10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="BC10" s="5" t="s">
+      <c r="BJ11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="BD10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="BE10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="BF10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="BG10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="BH10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="BI10" s="5" t="s">
+      <c r="BK11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="BJ10" s="5" t="s">
+      <c r="BL11" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="BK10" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
#4494-PurchaseInvoiceReport Module: pabi_account_report (Restart & Update Module) https://mobileapp.nstda.or.th/redmine/issues/4494
</commit_message>
<xml_diff>
--- a/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
+++ b/pabi_account_report/xlsx_template/xlsx_report_purchase_invoice_plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="68">
   <si>
     <t>PO Number</t>
   </si>
@@ -221,18 +221,22 @@
     <t>Invoice Status</t>
   </si>
   <si>
-    <t>Period</t>
-  </si>
-  <si>
     <t>Filter</t>
+  </si>
+  <si>
+    <t>Period Invoice</t>
+  </si>
+  <si>
+    <t>Period KV</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="187" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="188" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -294,7 +298,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -312,6 +316,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="188" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="188" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -599,58 +607,61 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:BL11"/>
+  <dimension ref="A1:BM11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="12.875" customWidth="1"/>
-    <col min="3" max="3" width="16.25" customWidth="1"/>
-    <col min="4" max="4" width="16.25" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.875" customWidth="1"/>
+    <col min="1" max="1" width="8.375" customWidth="1"/>
+    <col min="2" max="2" width="13.125" customWidth="1"/>
+    <col min="3" max="3" width="15.25" customWidth="1"/>
+    <col min="4" max="4" width="15.25" style="3" customWidth="1"/>
+    <col min="5" max="5" width="7.5" customWidth="1"/>
     <col min="6" max="7" width="16.25" customWidth="1"/>
     <col min="8" max="8" width="21.5" customWidth="1"/>
     <col min="9" max="9" width="16.25" customWidth="1"/>
-    <col min="10" max="10" width="23.375" customWidth="1"/>
+    <col min="10" max="10" width="19.875" customWidth="1"/>
     <col min="11" max="12" width="16.25" customWidth="1"/>
     <col min="13" max="13" width="16.25" style="2" customWidth="1"/>
     <col min="14" max="19" width="42.375" customWidth="1"/>
     <col min="20" max="20" width="16.25" customWidth="1"/>
     <col min="21" max="21" width="42.375" customWidth="1"/>
     <col min="22" max="22" width="16.25" customWidth="1"/>
-    <col min="23" max="24" width="42.375" customWidth="1"/>
+    <col min="23" max="23" width="42.375" customWidth="1"/>
+    <col min="24" max="24" width="23" customWidth="1"/>
     <col min="25" max="25" width="14.75" customWidth="1"/>
     <col min="26" max="26" width="13" customWidth="1"/>
     <col min="27" max="27" width="16.25" customWidth="1"/>
     <col min="28" max="28" width="13.875" customWidth="1"/>
     <col min="29" max="29" width="12.5" style="1" customWidth="1"/>
     <col min="30" max="30" width="42.375" style="1" customWidth="1"/>
-    <col min="31" max="31" width="16.25" customWidth="1"/>
-    <col min="32" max="33" width="16.25" style="1" customWidth="1"/>
-    <col min="34" max="41" width="16.25" customWidth="1"/>
-    <col min="42" max="43" width="19.5" customWidth="1"/>
-    <col min="44" max="45" width="16.25" customWidth="1"/>
-    <col min="46" max="46" width="16.625" customWidth="1"/>
-    <col min="47" max="47" width="17.875" customWidth="1"/>
-    <col min="48" max="54" width="16.25" customWidth="1"/>
-    <col min="55" max="55" width="21.875" customWidth="1"/>
-    <col min="56" max="56" width="17.875" customWidth="1"/>
-    <col min="57" max="58" width="16.25" customWidth="1"/>
-    <col min="59" max="59" width="9.875" customWidth="1"/>
-    <col min="60" max="60" width="23" customWidth="1"/>
-    <col min="61" max="61" width="10.25" customWidth="1"/>
-    <col min="62" max="62" width="16.25" customWidth="1"/>
-    <col min="63" max="63" width="9.75" customWidth="1"/>
+    <col min="31" max="32" width="16.25" customWidth="1"/>
+    <col min="33" max="34" width="16.25" style="1" customWidth="1"/>
+    <col min="35" max="39" width="16.25" customWidth="1"/>
+    <col min="40" max="40" width="16.25" style="9" customWidth="1"/>
+    <col min="41" max="42" width="16.25" customWidth="1"/>
+    <col min="43" max="44" width="19.5" customWidth="1"/>
+    <col min="45" max="46" width="16.25" customWidth="1"/>
+    <col min="47" max="47" width="16.625" customWidth="1"/>
+    <col min="48" max="48" width="17.875" customWidth="1"/>
+    <col min="49" max="55" width="16.25" customWidth="1"/>
+    <col min="56" max="56" width="21.875" customWidth="1"/>
+    <col min="57" max="57" width="17.875" style="9" customWidth="1"/>
+    <col min="58" max="59" width="16.25" customWidth="1"/>
+    <col min="60" max="60" width="9.875" customWidth="1"/>
+    <col min="61" max="61" width="23" customWidth="1"/>
+    <col min="62" max="62" width="10.25" customWidth="1"/>
+    <col min="63" max="63" width="16.25" customWidth="1"/>
+    <col min="64" max="64" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>45</v>
       </c>
@@ -661,8 +672,9 @@
       <c r="AC2"/>
       <c r="AD2"/>
       <c r="AE2" s="1"/>
-    </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="AF2" s="1"/>
+    </row>
+    <row r="3" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -675,8 +687,9 @@
       <c r="AC3"/>
       <c r="AD3"/>
       <c r="AE3" s="1"/>
-    </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="AF3" s="1"/>
+    </row>
+    <row r="4" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -689,8 +702,9 @@
       <c r="AC4"/>
       <c r="AD4"/>
       <c r="AE4" s="1"/>
-    </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="AF4" s="1"/>
+    </row>
+    <row r="5" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -703,8 +717,9 @@
       <c r="AC5"/>
       <c r="AD5"/>
       <c r="AE5" s="1"/>
-    </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="AF5" s="1"/>
+    </row>
+    <row r="6" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>37</v>
       </c>
@@ -717,8 +732,9 @@
       <c r="AC6"/>
       <c r="AD6"/>
       <c r="AE6" s="1"/>
-    </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="AF6" s="1"/>
+    </row>
+    <row r="7" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>47</v>
       </c>
@@ -729,8 +745,9 @@
       <c r="AC7"/>
       <c r="AD7"/>
       <c r="AE7" s="1"/>
-    </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="AF7" s="1"/>
+    </row>
+    <row r="8" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -741,10 +758,11 @@
       <c r="AC8"/>
       <c r="AD8"/>
       <c r="AE8" s="1"/>
-    </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="AF8" s="1"/>
+    </row>
+    <row r="9" spans="1:65" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
@@ -753,8 +771,9 @@
       <c r="AC9"/>
       <c r="AD9"/>
       <c r="AE9" s="1"/>
-    </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="AF9" s="1"/>
+    </row>
+    <row r="10" spans="1:65" x14ac:dyDescent="0.2">
       <c r="Y10" s="1"/>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1"/>
@@ -762,8 +781,9 @@
       <c r="AC10"/>
       <c r="AD10"/>
       <c r="AE10" s="1"/>
-    </row>
-    <row r="11" spans="1:64" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="AF10" s="1"/>
+    </row>
+    <row r="11" spans="1:65" s="5" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
@@ -857,103 +877,106 @@
       <c r="AE11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AF11" s="8" t="s">
+      <c r="AF11" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="AG11" s="8" t="s">
+      <c r="AH11" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="AH11" s="8" t="s">
+      <c r="AI11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AI11" s="5" t="s">
+      <c r="AJ11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AJ11" s="8" t="s">
+      <c r="AK11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AK11" s="8" t="s">
+      <c r="AL11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="AL11" s="5" t="s">
+      <c r="AM11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AM11" s="8" t="s">
+      <c r="AN11" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="AN11" s="5" t="s">
+      <c r="AO11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AO11" s="5" t="s">
+      <c r="AP11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AP11" s="5" t="s">
+      <c r="AQ11" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AQ11" s="5" t="s">
+      <c r="AR11" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AR11" s="5" t="s">
+      <c r="AS11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AS11" s="5" t="s">
+      <c r="AT11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AT11" s="5" t="s">
+      <c r="AU11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AU11" s="5" t="s">
+      <c r="AV11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AV11" s="5" t="s">
+      <c r="AW11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AW11" s="5" t="s">
+      <c r="AX11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AX11" s="5" t="s">
+      <c r="AY11" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AY11" s="5" t="s">
+      <c r="AZ11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AZ11" s="5" t="s">
+      <c r="BA11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="BA11" s="5" t="s">
+      <c r="BB11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="BB11" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="BC11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="BD11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="BD11" s="5" t="s">
+      <c r="BE11" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="BE11" s="5" t="s">
+      <c r="BF11" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="BF11" s="5" t="s">
+      <c r="BG11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="BG11" s="5" t="s">
+      <c r="BH11" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="BH11" s="5" t="s">
+      <c r="BI11" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BI11" s="5" t="s">
+      <c r="BJ11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="BJ11" s="5" t="s">
+      <c r="BK11" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="BK11" s="5" t="s">
+      <c r="BL11" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="BL11" s="5" t="s">
+      <c r="BM11" s="5" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>